<commit_message>
Add wild rubber dandelion.
Took 4 hours 6 minutes
</commit_message>
<xml_diff>
--- a/src/datagen/resources/data/frostedheart/data/plant_temperature.xlsx
+++ b/src/datagen/resources/data/frostedheart/data/plant_temperature.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyc/Development/FrostedHeart/src/datagen/resources/data/frostedheart/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\java\mcmod\1.20.1\FrostedHeart\src\datagen\resources\data\frostedheart\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E48E812-4CB2-CC4C-9259-A89D1ADDACA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439AD719-FCB4-44F9-BBB9-D1E35DDE66BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8120" yWindow="760" windowWidth="22120" windowHeight="17980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="110">
   <si>
     <t>block</t>
   </si>
@@ -347,13 +347,17 @@
   </si>
   <si>
     <t>frostedheart:rubber_dandelion</t>
+  </si>
+  <si>
+    <t>frostedheart:wild_rubber_dandelion</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -387,6 +391,12 @@
       <color rgb="FF000000"/>
       <name val="等线"/>
       <family val="4"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -441,7 +451,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -753,25 +763,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K95"/>
+  <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="176" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96:XFD96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="23.625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="5" customWidth="1"/>
     <col min="3" max="3" width="12" style="5" customWidth="1"/>
     <col min="4" max="4" width="9" style="5"/>
-    <col min="5" max="5" width="9.1640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.875" style="5" customWidth="1"/>
     <col min="8" max="8" width="12.5" style="5" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="28.33203125" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="28.375" customWidth="1"/>
+    <col min="11" max="11" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" customHeight="1">
@@ -4099,7 +4109,43 @@
         <v>1</v>
       </c>
     </row>
+    <row r="96" spans="1:11">
+      <c r="A96" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B96" s="5">
+        <v>14</v>
+      </c>
+      <c r="C96" s="5">
+        <v>22</v>
+      </c>
+      <c r="D96" s="5">
+        <v>6</v>
+      </c>
+      <c r="E96" s="5">
+        <v>26</v>
+      </c>
+      <c r="F96" s="5">
+        <v>-20</v>
+      </c>
+      <c r="G96" s="5">
+        <v>30</v>
+      </c>
+      <c r="H96" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I96" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J96" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K96" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adjust some temperature details
Took 1 hour 27 minutes
</commit_message>
<xml_diff>
--- a/src/datagen/resources/data/frostedheart/data/plant_temperature.xlsx
+++ b/src/datagen/resources/data/frostedheart/data/plant_temperature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\java\mcmod\1.20.1\FrostedHeart\src\datagen\resources\data\frostedheart\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439AD719-FCB4-44F9-BBB9-D1E35DDE66BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC82ACBF-9B80-4001-8912-D2F7A707957B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -220,9 +220,6 @@
     <t>minecraft:twisting_vines</t>
   </si>
   <si>
-    <t>minecraft:vines</t>
-  </si>
-  <si>
     <t>minecraft:tall_grass</t>
   </si>
   <si>
@@ -350,6 +347,10 @@
   </si>
   <si>
     <t>frostedheart:wild_rubber_dandelion</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>minecraft:vine</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -765,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96:XFD96"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2536,7 +2537,7 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="5" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="B51" s="5">
         <v>22</v>
@@ -2571,7 +2572,7 @@
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B52" s="5">
         <v>16</v>
@@ -2606,7 +2607,7 @@
     </row>
     <row r="53" spans="1:11">
       <c r="A53" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B53" s="5">
         <v>14</v>
@@ -2641,7 +2642,7 @@
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B54" s="5">
         <v>20</v>
@@ -2676,7 +2677,7 @@
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B55" s="5">
         <v>14</v>
@@ -2711,7 +2712,7 @@
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B56" s="5">
         <v>16</v>
@@ -2746,7 +2747,7 @@
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B57" s="5">
         <v>14</v>
@@ -2781,7 +2782,7 @@
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B58" s="5">
         <v>18</v>
@@ -2816,7 +2817,7 @@
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B59" s="5">
         <v>22</v>
@@ -2851,7 +2852,7 @@
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B60" s="5">
         <v>22</v>
@@ -2886,7 +2887,7 @@
     </row>
     <row r="61" spans="1:11">
       <c r="A61" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B61" s="5">
         <v>6</v>
@@ -2956,7 +2957,7 @@
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B63" s="5">
         <v>24</v>
@@ -2991,7 +2992,7 @@
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B64" s="5">
         <v>18</v>
@@ -3026,7 +3027,7 @@
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B65" s="5">
         <v>20</v>
@@ -3061,7 +3062,7 @@
     </row>
     <row r="66" spans="1:11">
       <c r="A66" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B66" s="5">
         <v>18</v>
@@ -3096,7 +3097,7 @@
     </row>
     <row r="67" spans="1:11">
       <c r="A67" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B67" s="5">
         <v>22</v>
@@ -3131,7 +3132,7 @@
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B68" s="5">
         <v>10</v>
@@ -3166,7 +3167,7 @@
     </row>
     <row r="69" spans="1:11">
       <c r="A69" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B69" s="5">
         <v>14</v>
@@ -3201,7 +3202,7 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B70" s="5">
         <v>16</v>
@@ -3271,7 +3272,7 @@
     </row>
     <row r="72" spans="1:11">
       <c r="A72" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B72" s="5">
         <v>18</v>
@@ -3306,7 +3307,7 @@
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B73" s="5">
         <v>18</v>
@@ -3341,7 +3342,7 @@
     </row>
     <row r="74" spans="1:11">
       <c r="A74" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B74" s="5">
         <v>18</v>
@@ -3376,7 +3377,7 @@
     </row>
     <row r="75" spans="1:11">
       <c r="A75" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B75" s="5">
         <v>20</v>
@@ -3411,7 +3412,7 @@
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B76" s="5">
         <v>22</v>
@@ -3446,7 +3447,7 @@
     </row>
     <row r="77" spans="1:11">
       <c r="A77" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B77" s="5">
         <v>24</v>
@@ -3481,7 +3482,7 @@
     </row>
     <row r="78" spans="1:11">
       <c r="A78" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B78" s="5">
         <v>18</v>
@@ -3516,7 +3517,7 @@
     </row>
     <row r="79" spans="1:11">
       <c r="A79" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B79" s="5">
         <v>20</v>
@@ -3551,7 +3552,7 @@
     </row>
     <row r="80" spans="1:11">
       <c r="A80" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B80" s="5">
         <v>22</v>
@@ -3586,7 +3587,7 @@
     </row>
     <row r="81" spans="1:11">
       <c r="A81" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B81" s="5">
         <v>20</v>
@@ -3621,7 +3622,7 @@
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B82" s="5">
         <v>22</v>
@@ -3656,7 +3657,7 @@
     </row>
     <row r="83" spans="1:11">
       <c r="A83" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B83" s="5">
         <v>24</v>
@@ -3691,7 +3692,7 @@
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B84" s="5">
         <v>18</v>
@@ -3726,7 +3727,7 @@
     </row>
     <row r="85" spans="1:11">
       <c r="A85" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B85" s="5">
         <v>18</v>
@@ -3761,7 +3762,7 @@
     </row>
     <row r="86" spans="1:11">
       <c r="A86" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B86" s="5">
         <v>30</v>
@@ -3796,7 +3797,7 @@
     </row>
     <row r="87" spans="1:11">
       <c r="A87" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B87" s="5">
         <v>20</v>
@@ -3831,7 +3832,7 @@
     </row>
     <row r="88" spans="1:11">
       <c r="A88" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B88" s="5">
         <v>16</v>
@@ -3866,7 +3867,7 @@
     </row>
     <row r="89" spans="1:11">
       <c r="A89" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B89" s="5">
         <v>22</v>
@@ -3901,7 +3902,7 @@
     </row>
     <row r="90" spans="1:11">
       <c r="A90" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B90" s="5">
         <v>12</v>
@@ -3936,7 +3937,7 @@
     </row>
     <row r="91" spans="1:11">
       <c r="A91" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B91" s="5">
         <v>12</v>
@@ -3971,7 +3972,7 @@
     </row>
     <row r="92" spans="1:11">
       <c r="A92" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B92" s="5">
         <v>16</v>
@@ -4006,7 +4007,7 @@
     </row>
     <row r="93" spans="1:11">
       <c r="A93" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B93" s="5">
         <v>22</v>
@@ -4041,7 +4042,7 @@
     </row>
     <row r="94" spans="1:11">
       <c r="A94" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B94" s="5">
         <v>18</v>
@@ -4076,7 +4077,7 @@
     </row>
     <row r="95" spans="1:11">
       <c r="A95" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B95" s="5">
         <v>14</v>
@@ -4111,7 +4112,7 @@
     </row>
     <row r="96" spans="1:11">
       <c r="A96" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B96" s="5">
         <v>14</v>

</xml_diff>

<commit_message>
Animal hides, meats, clothes, and datagen
</commit_message>
<xml_diff>
--- a/src/datagen/resources/data/frostedheart/data/plant_temperature.xlsx
+++ b/src/datagen/resources/data/frostedheart/data/plant_temperature.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyc/Development/FrostedHeart/src/datagen/resources/data/frostedheart/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F783C86-2F63-7B40-888A-5443F4990B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE9A7B4-CFBE-5742-B9C5-3D32BB7597F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="109">
   <si>
     <t>block</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>frostedheart:white_turnip_block</t>
-  </si>
-  <si>
-    <t>frostedheart:wolfberry_bush_block</t>
   </si>
   <si>
     <t>minecraft:moss_block</t>
@@ -764,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K96"/>
+  <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -814,10 +811,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.25" customHeight="1">
@@ -849,7 +846,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K2" t="b">
         <v>1</v>
@@ -884,38 +881,38 @@
         <v>0</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K3" s="7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.25" customHeight="1">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:11">
+      <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2">
-        <v>26</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="B4" s="5">
         <v>10</v>
       </c>
-      <c r="E4" s="2">
-        <v>30</v>
-      </c>
-      <c r="F4" s="2">
-        <v>-10</v>
-      </c>
-      <c r="G4" s="2">
-        <v>35</v>
-      </c>
-      <c r="H4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2" t="b">
+      <c r="C4" s="5">
+        <v>50</v>
+      </c>
+      <c r="D4" s="5">
+        <v>5</v>
+      </c>
+      <c r="E4" s="5">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>50</v>
+      </c>
+      <c r="H4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5" t="b">
         <v>1</v>
       </c>
       <c r="J4" s="6" t="s">
@@ -927,34 +924,34 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B5" s="5">
+        <v>20</v>
+      </c>
+      <c r="C5" s="5">
+        <v>40</v>
+      </c>
+      <c r="D5" s="5">
         <v>10</v>
       </c>
-      <c r="C5" s="5">
-        <v>50</v>
-      </c>
-      <c r="D5" s="5">
-        <v>5</v>
-      </c>
       <c r="E5" s="5">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F5" s="5">
         <v>0</v>
       </c>
       <c r="G5" s="5">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H5" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I5" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K5" s="7" t="b">
         <v>1</v>
@@ -962,37 +959,37 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B6" s="5">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="C6" s="5">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="D6" s="5">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E6" s="5">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="F6" s="5">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G6" s="5">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H6" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I6" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="7" t="b">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="K6" s="8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1018,16 +1015,16 @@
         <v>200</v>
       </c>
       <c r="H7" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="8" t="b">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="K7" s="7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1059,7 +1056,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K8" s="7" t="b">
         <v>1</v>
@@ -1070,22 +1067,22 @@
         <v>17</v>
       </c>
       <c r="B9" s="5">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C9" s="5">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="D9" s="5">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="E9" s="5">
-        <v>200</v>
+        <v>35</v>
       </c>
       <c r="F9" s="5">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G9" s="5">
-        <v>200</v>
+        <v>35</v>
       </c>
       <c r="H9" s="5" t="b">
         <v>0</v>
@@ -1094,77 +1091,77 @@
         <v>0</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="K9" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B10" s="5">
         <v>20</v>
       </c>
       <c r="C10" s="5">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D10" s="5">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E10" s="5">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F10" s="5">
         <v>0</v>
       </c>
       <c r="G10" s="5">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="H10" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K10" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="4" t="s">
-        <v>25</v>
+      <c r="A11" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B11" s="5">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C11" s="5">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D11" s="5">
         <v>10</v>
       </c>
       <c r="E11" s="5">
+        <v>32</v>
+      </c>
+      <c r="F11" s="5">
+        <v>-10</v>
+      </c>
+      <c r="G11" s="5">
         <v>40</v>
       </c>
-      <c r="F11" s="5">
-        <v>0</v>
-      </c>
-      <c r="G11" s="5">
-        <v>50</v>
-      </c>
       <c r="H11" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="K11" s="7" t="b">
         <v>1</v>
@@ -1175,31 +1172,31 @@
         <v>27</v>
       </c>
       <c r="B12" s="5">
+        <v>-2</v>
+      </c>
+      <c r="C12" s="5">
         <v>12</v>
       </c>
-      <c r="C12" s="5">
-        <v>24</v>
-      </c>
       <c r="D12" s="5">
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="E12" s="5">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="F12" s="5">
-        <v>-10</v>
+        <v>-40</v>
       </c>
       <c r="G12" s="5">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="H12" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K12" s="7" t="b">
         <v>1</v>
@@ -1210,22 +1207,22 @@
         <v>28</v>
       </c>
       <c r="B13" s="5">
-        <v>-2</v>
+        <v>8</v>
       </c>
       <c r="C13" s="5">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D13" s="5">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="E13" s="5">
         <v>22</v>
       </c>
       <c r="F13" s="5">
-        <v>-40</v>
+        <v>-25</v>
       </c>
       <c r="G13" s="5">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="H13" s="5" t="b">
         <v>1</v>
@@ -1234,7 +1231,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K13" s="7" t="b">
         <v>1</v>
@@ -1245,31 +1242,31 @@
         <v>29</v>
       </c>
       <c r="B14" s="5">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C14" s="5">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D14" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E14" s="5">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="F14" s="5">
-        <v>-25</v>
+        <v>10</v>
       </c>
       <c r="G14" s="5">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="H14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K14" s="7" t="b">
         <v>1</v>
@@ -1280,7 +1277,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="5">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="5">
         <v>32</v>
@@ -1292,10 +1289,10 @@
         <v>42</v>
       </c>
       <c r="F15" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G15" s="5">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H15" s="5" t="b">
         <v>0</v>
@@ -1304,7 +1301,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K15" s="7" t="b">
         <v>1</v>
@@ -1315,22 +1312,22 @@
         <v>31</v>
       </c>
       <c r="B16" s="5">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C16" s="5">
+        <v>26</v>
+      </c>
+      <c r="D16" s="5">
+        <v>10</v>
+      </c>
+      <c r="E16" s="5">
         <v>32</v>
       </c>
-      <c r="D16" s="5">
-        <v>20</v>
-      </c>
-      <c r="E16" s="5">
-        <v>42</v>
-      </c>
       <c r="F16" s="5">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="G16" s="5">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H16" s="5" t="b">
         <v>0</v>
@@ -1339,7 +1336,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K16" s="7" t="b">
         <v>1</v>
@@ -1350,22 +1347,22 @@
         <v>32</v>
       </c>
       <c r="B17" s="5">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C17" s="5">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D17" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E17" s="5">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F17" s="5">
-        <v>-5</v>
+        <v>15</v>
       </c>
       <c r="G17" s="5">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="H17" s="5" t="b">
         <v>0</v>
@@ -1374,7 +1371,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K17" s="7" t="b">
         <v>1</v>
@@ -1385,31 +1382,31 @@
         <v>33</v>
       </c>
       <c r="B18" s="5">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C18" s="5">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D18" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E18" s="5">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="F18" s="5">
-        <v>15</v>
+        <v>-20</v>
       </c>
       <c r="G18" s="5">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H18" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="5" t="b">
         <v>0</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K18" s="7" t="b">
         <v>1</v>
@@ -1420,10 +1417,10 @@
         <v>34</v>
       </c>
       <c r="B19" s="5">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C19" s="5">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D19" s="5">
         <v>10</v>
@@ -1432,10 +1429,10 @@
         <v>32</v>
       </c>
       <c r="F19" s="5">
-        <v>-20</v>
+        <v>-10</v>
       </c>
       <c r="G19" s="5">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H19" s="5" t="b">
         <v>1</v>
@@ -1444,7 +1441,7 @@
         <v>0</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K19" s="7" t="b">
         <v>1</v>
@@ -1479,7 +1476,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K20" s="7" t="b">
         <v>1</v>
@@ -1490,31 +1487,31 @@
         <v>36</v>
       </c>
       <c r="B21" s="5">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C21" s="5">
+        <v>20</v>
+      </c>
+      <c r="D21" s="5">
+        <v>2</v>
+      </c>
+      <c r="E21" s="5">
         <v>24</v>
       </c>
-      <c r="D21" s="5">
-        <v>10</v>
-      </c>
-      <c r="E21" s="5">
-        <v>32</v>
-      </c>
       <c r="F21" s="5">
-        <v>-10</v>
+        <v>-50</v>
       </c>
       <c r="G21" s="5">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H21" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I21" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K21" s="7" t="b">
         <v>1</v>
@@ -1549,42 +1546,42 @@
         <v>1</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K22" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B23" s="5">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="C23" s="5">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="D23" s="5">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="E23" s="5">
-        <v>24</v>
+        <v>200</v>
       </c>
       <c r="F23" s="5">
-        <v>-50</v>
+        <v>80</v>
       </c>
       <c r="G23" s="5">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="H23" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K23" s="7" t="b">
         <v>1</v>
@@ -1619,42 +1616,42 @@
         <v>0</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K24" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B25" s="5">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="C25" s="5">
-        <v>200</v>
+        <v>28</v>
       </c>
       <c r="D25" s="5">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="E25" s="5">
-        <v>200</v>
+        <v>32</v>
       </c>
       <c r="F25" s="5">
-        <v>80</v>
+        <v>-10</v>
       </c>
       <c r="G25" s="5">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="H25" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K25" s="7" t="b">
         <v>1</v>
@@ -1665,31 +1662,31 @@
         <v>41</v>
       </c>
       <c r="B26" s="5">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C26" s="5">
+        <v>24</v>
+      </c>
+      <c r="D26" s="5">
+        <v>8</v>
+      </c>
+      <c r="E26" s="5">
         <v>28</v>
       </c>
-      <c r="D26" s="5">
-        <v>10</v>
-      </c>
-      <c r="E26" s="5">
-        <v>32</v>
-      </c>
       <c r="F26" s="5">
-        <v>-10</v>
+        <v>-5</v>
       </c>
       <c r="G26" s="5">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H26" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I26" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K26" s="7" t="b">
         <v>1</v>
@@ -1703,28 +1700,28 @@
         <v>14</v>
       </c>
       <c r="C27" s="5">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D27" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E27" s="5">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F27" s="5">
-        <v>-5</v>
+        <v>-20</v>
       </c>
       <c r="G27" s="5">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H27" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I27" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K27" s="7" t="b">
         <v>1</v>
@@ -1735,31 +1732,31 @@
         <v>43</v>
       </c>
       <c r="B28" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C28" s="5">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D28" s="5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E28" s="5">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F28" s="5">
-        <v>-20</v>
+        <v>-5</v>
       </c>
       <c r="G28" s="5">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H28" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K28" s="7" t="b">
         <v>1</v>
@@ -1770,19 +1767,19 @@
         <v>44</v>
       </c>
       <c r="B29" s="5">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C29" s="5">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D29" s="5">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E29" s="5">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F29" s="5">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="G29" s="5">
         <v>35</v>
@@ -1794,7 +1791,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K29" s="7" t="b">
         <v>1</v>
@@ -1805,31 +1802,31 @@
         <v>45</v>
       </c>
       <c r="B30" s="5">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C30" s="5">
+        <v>22</v>
+      </c>
+      <c r="D30" s="5">
+        <v>8</v>
+      </c>
+      <c r="E30" s="5">
         <v>26</v>
       </c>
-      <c r="D30" s="5">
-        <v>14</v>
-      </c>
-      <c r="E30" s="5">
-        <v>30</v>
-      </c>
       <c r="F30" s="5">
-        <v>5</v>
+        <v>-10</v>
       </c>
       <c r="G30" s="5">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H30" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" s="5" t="b">
         <v>0</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K30" s="7" t="b">
         <v>1</v>
@@ -1840,31 +1837,31 @@
         <v>46</v>
       </c>
       <c r="B31" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C31" s="5">
         <v>22</v>
       </c>
       <c r="D31" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E31" s="5">
         <v>26</v>
       </c>
       <c r="F31" s="5">
-        <v>-10</v>
+        <v>-5</v>
       </c>
       <c r="G31" s="5">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H31" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31" s="5" t="b">
         <v>0</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K31" s="7" t="b">
         <v>1</v>
@@ -1875,31 +1872,31 @@
         <v>47</v>
       </c>
       <c r="B32" s="5">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C32" s="5">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D32" s="5">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E32" s="5">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F32" s="5">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="G32" s="5">
         <v>30</v>
       </c>
       <c r="H32" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="5" t="b">
         <v>0</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K32" s="7" t="b">
         <v>1</v>
@@ -1934,7 +1931,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K33" s="7" t="b">
         <v>1</v>
@@ -1969,7 +1966,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K34" s="7" t="b">
         <v>1</v>
@@ -2004,7 +2001,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K35" s="7" t="b">
         <v>1</v>
@@ -2015,22 +2012,22 @@
         <v>51</v>
       </c>
       <c r="B36" s="5">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C36" s="5">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D36" s="5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E36" s="5">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F36" s="5">
-        <v>-15</v>
+        <v>-10</v>
       </c>
       <c r="G36" s="5">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H36" s="5" t="b">
         <v>1</v>
@@ -2039,7 +2036,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K36" s="7" t="b">
         <v>1</v>
@@ -2050,22 +2047,22 @@
         <v>52</v>
       </c>
       <c r="B37" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C37" s="5">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D37" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E37" s="5">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F37" s="5">
         <v>-10</v>
       </c>
       <c r="G37" s="5">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H37" s="5" t="b">
         <v>1</v>
@@ -2074,7 +2071,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K37" s="7" t="b">
         <v>1</v>
@@ -2085,31 +2082,31 @@
         <v>53</v>
       </c>
       <c r="B38" s="5">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C38" s="5">
+        <v>20</v>
+      </c>
+      <c r="D38" s="5">
+        <v>6</v>
+      </c>
+      <c r="E38" s="5">
         <v>24</v>
       </c>
-      <c r="D38" s="5">
-        <v>10</v>
-      </c>
-      <c r="E38" s="5">
-        <v>28</v>
-      </c>
       <c r="F38" s="5">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="G38" s="5">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H38" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I38" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K38" s="7" t="b">
         <v>1</v>
@@ -2120,31 +2117,31 @@
         <v>54</v>
       </c>
       <c r="B39" s="5">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C39" s="5">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D39" s="5">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E39" s="5">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F39" s="5">
-        <v>-20</v>
+        <v>5</v>
       </c>
       <c r="G39" s="5">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="H39" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K39" s="7" t="b">
         <v>1</v>
@@ -2155,31 +2152,31 @@
         <v>55</v>
       </c>
       <c r="B40" s="5">
-        <v>22</v>
+        <v>-100</v>
       </c>
       <c r="C40" s="5">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="D40" s="5">
-        <v>16</v>
+        <v>-100</v>
       </c>
       <c r="E40" s="5">
-        <v>36</v>
+        <v>100</v>
       </c>
       <c r="F40" s="5">
-        <v>5</v>
+        <v>-100</v>
       </c>
       <c r="G40" s="5">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="H40" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K40" s="7" t="b">
         <v>1</v>
@@ -2190,31 +2187,31 @@
         <v>56</v>
       </c>
       <c r="B41" s="5">
-        <v>-100</v>
+        <v>12</v>
       </c>
       <c r="C41" s="5">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="D41" s="5">
-        <v>-100</v>
+        <v>8</v>
       </c>
       <c r="E41" s="5">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="F41" s="5">
-        <v>-100</v>
+        <v>-20</v>
       </c>
       <c r="G41" s="5">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="H41" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I41" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K41" s="7" t="b">
         <v>1</v>
@@ -2225,31 +2222,31 @@
         <v>57</v>
       </c>
       <c r="B42" s="5">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C42" s="5">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D42" s="5">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E42" s="5">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F42" s="5">
-        <v>-20</v>
+        <v>5</v>
       </c>
       <c r="G42" s="5">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="H42" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" s="5" t="b">
         <v>0</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K42" s="7" t="b">
         <v>1</v>
@@ -2260,19 +2257,19 @@
         <v>58</v>
       </c>
       <c r="B43" s="5">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C43" s="5">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D43" s="5">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E43" s="5">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F43" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G43" s="5">
         <v>42</v>
@@ -2284,7 +2281,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K43" s="7" t="b">
         <v>1</v>
@@ -2295,22 +2292,22 @@
         <v>59</v>
       </c>
       <c r="B44" s="5">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C44" s="5">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D44" s="5">
         <v>20</v>
       </c>
       <c r="E44" s="5">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="F44" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G44" s="5">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="H44" s="5" t="b">
         <v>0</v>
@@ -2319,33 +2316,33 @@
         <v>0</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K44" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:11">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="4" t="s">
         <v>60</v>
       </c>
       <c r="B45" s="5">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="C45" s="5">
-        <v>38</v>
+        <v>200</v>
       </c>
       <c r="D45" s="5">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E45" s="5">
-        <v>45</v>
+        <v>200</v>
       </c>
       <c r="F45" s="5">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="G45" s="5">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="H45" s="5" t="b">
         <v>0</v>
@@ -2354,7 +2351,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K45" s="7" t="b">
         <v>1</v>
@@ -2389,42 +2386,42 @@
         <v>0</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K46" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:11">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="10">
         <v>80</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="10">
         <v>200</v>
       </c>
-      <c r="D47" s="5">
+      <c r="D47" s="10">
         <v>80</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E47" s="10">
         <v>200</v>
       </c>
-      <c r="F47" s="5">
+      <c r="F47" s="10">
         <v>80</v>
       </c>
-      <c r="G47" s="5">
+      <c r="G47" s="10">
         <v>200</v>
       </c>
-      <c r="H47" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I47" s="5" t="b">
+      <c r="H47" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" s="10" t="b">
         <v>0</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K47" s="7" t="b">
         <v>1</v>
@@ -2459,7 +2456,7 @@
         <v>0</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K48" s="7" t="b">
         <v>1</v>
@@ -2494,42 +2491,42 @@
         <v>0</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K49" s="7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B50" s="10">
-        <v>80</v>
-      </c>
-      <c r="C50" s="10">
-        <v>200</v>
-      </c>
-      <c r="D50" s="10">
-        <v>80</v>
-      </c>
-      <c r="E50" s="10">
-        <v>200</v>
-      </c>
-      <c r="F50" s="10">
-        <v>80</v>
-      </c>
-      <c r="G50" s="10">
-        <v>200</v>
-      </c>
-      <c r="H50" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I50" s="10" t="b">
+      <c r="A50" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="5">
+        <v>22</v>
+      </c>
+      <c r="C50" s="5">
+        <v>30</v>
+      </c>
+      <c r="D50" s="5">
+        <v>16</v>
+      </c>
+      <c r="E50" s="5">
+        <v>34</v>
+      </c>
+      <c r="F50" s="5">
+        <v>5</v>
+      </c>
+      <c r="G50" s="5">
+        <v>38</v>
+      </c>
+      <c r="H50" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I50" s="5" t="b">
         <v>0</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K50" s="7" t="b">
         <v>1</v>
@@ -2537,34 +2534,34 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="5" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="B51" s="5">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C51" s="5">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D51" s="5">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E51" s="5">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F51" s="5">
-        <v>5</v>
+        <v>-10</v>
       </c>
       <c r="G51" s="5">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H51" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I51" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K51" s="7" t="b">
         <v>1</v>
@@ -2575,31 +2572,31 @@
         <v>66</v>
       </c>
       <c r="B52" s="5">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C52" s="5">
+        <v>24</v>
+      </c>
+      <c r="D52" s="5">
+        <v>8</v>
+      </c>
+      <c r="E52" s="5">
         <v>28</v>
       </c>
-      <c r="D52" s="5">
-        <v>10</v>
-      </c>
-      <c r="E52" s="5">
-        <v>32</v>
-      </c>
       <c r="F52" s="5">
-        <v>-10</v>
+        <v>-5</v>
       </c>
       <c r="G52" s="5">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H52" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I52" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K52" s="7" t="b">
         <v>1</v>
@@ -2610,31 +2607,31 @@
         <v>67</v>
       </c>
       <c r="B53" s="5">
+        <v>20</v>
+      </c>
+      <c r="C53" s="5">
+        <v>28</v>
+      </c>
+      <c r="D53" s="5">
         <v>14</v>
       </c>
-      <c r="C53" s="5">
-        <v>24</v>
-      </c>
-      <c r="D53" s="5">
-        <v>8</v>
-      </c>
       <c r="E53" s="5">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F53" s="5">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="G53" s="5">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H53" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" s="5" t="b">
         <v>0</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K53" s="7" t="b">
         <v>1</v>
@@ -2645,31 +2642,31 @@
         <v>68</v>
       </c>
       <c r="B54" s="5">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C54" s="5">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D54" s="5">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E54" s="5">
+        <v>26</v>
+      </c>
+      <c r="F54" s="5">
+        <v>-15</v>
+      </c>
+      <c r="G54" s="5">
         <v>32</v>
       </c>
-      <c r="F54" s="5">
-        <v>5</v>
-      </c>
-      <c r="G54" s="5">
-        <v>38</v>
-      </c>
       <c r="H54" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I54" s="5" t="b">
         <v>0</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K54" s="7" t="b">
         <v>1</v>
@@ -2680,22 +2677,22 @@
         <v>69</v>
       </c>
       <c r="B55" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C55" s="5">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D55" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E55" s="5">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F55" s="5">
-        <v>-15</v>
+        <v>-10</v>
       </c>
       <c r="G55" s="5">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H55" s="5" t="b">
         <v>1</v>
@@ -2704,7 +2701,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K55" s="7" t="b">
         <v>1</v>
@@ -2715,22 +2712,22 @@
         <v>70</v>
       </c>
       <c r="B56" s="5">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C56" s="5">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D56" s="5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E56" s="5">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F56" s="5">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="G56" s="5">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H56" s="5" t="b">
         <v>1</v>
@@ -2739,7 +2736,7 @@
         <v>0</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K56" s="7" t="b">
         <v>1</v>
@@ -2750,31 +2747,31 @@
         <v>71</v>
       </c>
       <c r="B57" s="5">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C57" s="5">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D57" s="5">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E57" s="5">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F57" s="5">
-        <v>-20</v>
+        <v>5</v>
       </c>
       <c r="G57" s="5">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H57" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57" s="5" t="b">
         <v>0</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K57" s="7" t="b">
         <v>1</v>
@@ -2785,22 +2782,22 @@
         <v>72</v>
       </c>
       <c r="B58" s="5">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C58" s="5">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D58" s="5">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E58" s="5">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F58" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G58" s="5">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H58" s="5" t="b">
         <v>0</v>
@@ -2809,7 +2806,7 @@
         <v>0</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K58" s="7" t="b">
         <v>1</v>
@@ -2844,7 +2841,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K59" s="7" t="b">
         <v>1</v>
@@ -2855,31 +2852,31 @@
         <v>74</v>
       </c>
       <c r="B60" s="5">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C60" s="5">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D60" s="5">
-        <v>16</v>
+        <v>-5</v>
       </c>
       <c r="E60" s="5">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F60" s="5">
-        <v>10</v>
+        <v>-40</v>
       </c>
       <c r="G60" s="5">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H60" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I60" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K60" s="7" t="b">
         <v>1</v>
@@ -2887,34 +2884,34 @@
     </row>
     <row r="61" spans="1:11">
       <c r="A61" s="5" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="B61" s="5">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C61" s="5">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D61" s="5">
+        <v>5</v>
+      </c>
+      <c r="E61" s="5">
+        <v>30</v>
+      </c>
+      <c r="F61" s="5">
         <v>-5</v>
       </c>
-      <c r="E61" s="5">
-        <v>24</v>
-      </c>
-      <c r="F61" s="5">
-        <v>-40</v>
-      </c>
       <c r="G61" s="5">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H61" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K61" s="7" t="b">
         <v>1</v>
@@ -2922,25 +2919,25 @@
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="5" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="B62" s="5">
+        <v>24</v>
+      </c>
+      <c r="C62" s="5">
+        <v>32</v>
+      </c>
+      <c r="D62" s="5">
+        <v>20</v>
+      </c>
+      <c r="E62" s="5">
+        <v>36</v>
+      </c>
+      <c r="F62" s="5">
         <v>15</v>
       </c>
-      <c r="C62" s="5">
-        <v>24</v>
-      </c>
-      <c r="D62" s="5">
-        <v>5</v>
-      </c>
-      <c r="E62" s="5">
-        <v>30</v>
-      </c>
-      <c r="F62" s="5">
-        <v>-5</v>
-      </c>
       <c r="G62" s="5">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H62" s="5" t="b">
         <v>0</v>
@@ -2949,7 +2946,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K62" s="7" t="b">
         <v>1</v>
@@ -2960,31 +2957,31 @@
         <v>76</v>
       </c>
       <c r="B63" s="5">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C63" s="5">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D63" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E63" s="5">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F63" s="5">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G63" s="5">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H63" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I63" s="5" t="b">
         <v>0</v>
       </c>
       <c r="J63" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K63" s="7" t="b">
         <v>1</v>
@@ -2995,31 +2992,31 @@
         <v>77</v>
       </c>
       <c r="B64" s="5">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C64" s="5">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D64" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E64" s="5">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F64" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G64" s="5">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H64" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I64" s="5" t="b">
         <v>0</v>
       </c>
       <c r="J64" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K64" s="7" t="b">
         <v>1</v>
@@ -3030,22 +3027,22 @@
         <v>78</v>
       </c>
       <c r="B65" s="5">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C65" s="5">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D65" s="5">
         <v>12</v>
       </c>
       <c r="E65" s="5">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F65" s="5">
         <v>5</v>
       </c>
       <c r="G65" s="5">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H65" s="5" t="b">
         <v>0</v>
@@ -3054,7 +3051,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K65" s="7" t="b">
         <v>1</v>
@@ -3065,22 +3062,22 @@
         <v>79</v>
       </c>
       <c r="B66" s="5">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C66" s="5">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D66" s="5">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E66" s="5">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F66" s="5">
         <v>5</v>
       </c>
       <c r="G66" s="5">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="H66" s="5" t="b">
         <v>0</v>
@@ -3089,7 +3086,7 @@
         <v>0</v>
       </c>
       <c r="J66" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K66" s="7" t="b">
         <v>1</v>
@@ -3100,31 +3097,31 @@
         <v>80</v>
       </c>
       <c r="B67" s="5">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C67" s="5">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D67" s="5">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E67" s="5">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F67" s="5">
-        <v>5</v>
+        <v>-20</v>
       </c>
       <c r="G67" s="5">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H67" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I67" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J67" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K67" s="7" t="b">
         <v>1</v>
@@ -3135,31 +3132,31 @@
         <v>81</v>
       </c>
       <c r="B68" s="5">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C68" s="5">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D68" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E68" s="5">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F68" s="5">
-        <v>-20</v>
+        <v>-2</v>
       </c>
       <c r="G68" s="5">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H68" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I68" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J68" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K68" s="7" t="b">
         <v>1</v>
@@ -3170,19 +3167,19 @@
         <v>82</v>
       </c>
       <c r="B69" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C69" s="5">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D69" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E69" s="5">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F69" s="5">
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="G69" s="5">
         <v>32</v>
@@ -3194,7 +3191,7 @@
         <v>0</v>
       </c>
       <c r="J69" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K69" s="7" t="b">
         <v>1</v>
@@ -3202,25 +3199,25 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="5" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="B70" s="5">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C70" s="5">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D70" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E70" s="5">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F70" s="5">
         <v>-5</v>
       </c>
       <c r="G70" s="5">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H70" s="5" t="b">
         <v>1</v>
@@ -3229,7 +3226,7 @@
         <v>0</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K70" s="7" t="b">
         <v>1</v>
@@ -3237,34 +3234,34 @@
     </row>
     <row r="71" spans="1:11">
       <c r="A71" s="5" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="B71" s="5">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C71" s="5">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D71" s="5">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E71" s="5">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F71" s="5">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="G71" s="5">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H71" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I71" s="5" t="b">
         <v>0</v>
       </c>
       <c r="J71" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K71" s="7" t="b">
         <v>1</v>
@@ -3278,19 +3275,19 @@
         <v>18</v>
       </c>
       <c r="C72" s="5">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D72" s="5">
         <v>12</v>
       </c>
       <c r="E72" s="5">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F72" s="5">
         <v>5</v>
       </c>
       <c r="G72" s="5">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H72" s="5" t="b">
         <v>0</v>
@@ -3299,7 +3296,7 @@
         <v>0</v>
       </c>
       <c r="J72" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K72" s="7" t="b">
         <v>1</v>
@@ -3334,7 +3331,7 @@
         <v>0</v>
       </c>
       <c r="J73" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K73" s="7" t="b">
         <v>1</v>
@@ -3345,22 +3342,22 @@
         <v>86</v>
       </c>
       <c r="B74" s="5">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C74" s="5">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D74" s="5">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E74" s="5">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F74" s="5">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="G74" s="5">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="H74" s="5" t="b">
         <v>0</v>
@@ -3369,7 +3366,7 @@
         <v>0</v>
       </c>
       <c r="J74" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K74" s="7" t="b">
         <v>1</v>
@@ -3380,22 +3377,22 @@
         <v>87</v>
       </c>
       <c r="B75" s="5">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C75" s="5">
         <v>30</v>
       </c>
       <c r="D75" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E75" s="5">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F75" s="5">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="G75" s="5">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H75" s="5" t="b">
         <v>0</v>
@@ -3404,7 +3401,7 @@
         <v>0</v>
       </c>
       <c r="J75" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K75" s="7" t="b">
         <v>1</v>
@@ -3415,19 +3412,19 @@
         <v>88</v>
       </c>
       <c r="B76" s="5">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C76" s="5">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D76" s="5">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E76" s="5">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F76" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G76" s="5">
         <v>38</v>
@@ -3439,7 +3436,7 @@
         <v>0</v>
       </c>
       <c r="J76" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K76" s="7" t="b">
         <v>1</v>
@@ -3450,31 +3447,31 @@
         <v>89</v>
       </c>
       <c r="B77" s="5">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C77" s="5">
+        <v>28</v>
+      </c>
+      <c r="D77" s="5">
+        <v>10</v>
+      </c>
+      <c r="E77" s="5">
         <v>32</v>
       </c>
-      <c r="D77" s="5">
-        <v>18</v>
-      </c>
-      <c r="E77" s="5">
-        <v>36</v>
-      </c>
       <c r="F77" s="5">
-        <v>5</v>
+        <v>-15</v>
       </c>
       <c r="G77" s="5">
         <v>38</v>
       </c>
       <c r="H77" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I77" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J77" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K77" s="7" t="b">
         <v>1</v>
@@ -3485,22 +3482,22 @@
         <v>90</v>
       </c>
       <c r="B78" s="5">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C78" s="5">
         <v>28</v>
       </c>
       <c r="D78" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E78" s="5">
         <v>32</v>
       </c>
       <c r="F78" s="5">
-        <v>-15</v>
+        <v>-5</v>
       </c>
       <c r="G78" s="5">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H78" s="5" t="b">
         <v>1</v>
@@ -3509,7 +3506,7 @@
         <v>1</v>
       </c>
       <c r="J78" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K78" s="7" t="b">
         <v>1</v>
@@ -3520,19 +3517,19 @@
         <v>91</v>
       </c>
       <c r="B79" s="5">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C79" s="5">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D79" s="5">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E79" s="5">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F79" s="5">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="G79" s="5">
         <v>36</v>
@@ -3541,10 +3538,10 @@
         <v>1</v>
       </c>
       <c r="I79" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J79" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K79" s="7" t="b">
         <v>1</v>
@@ -3555,31 +3552,31 @@
         <v>92</v>
       </c>
       <c r="B80" s="5">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C80" s="5">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D80" s="5">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E80" s="5">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F80" s="5">
-        <v>5</v>
+        <v>-20</v>
       </c>
       <c r="G80" s="5">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H80" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I80" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J80" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K80" s="7" t="b">
         <v>1</v>
@@ -3590,31 +3587,31 @@
         <v>93</v>
       </c>
       <c r="B81" s="5">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C81" s="5">
         <v>28</v>
       </c>
       <c r="D81" s="5">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E81" s="5">
         <v>32</v>
       </c>
       <c r="F81" s="5">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="G81" s="5">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H81" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I81" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J81" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K81" s="7" t="b">
         <v>1</v>
@@ -3625,19 +3622,19 @@
         <v>94</v>
       </c>
       <c r="B82" s="5">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C82" s="5">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D82" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E82" s="5">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F82" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G82" s="5">
         <v>36</v>
@@ -3649,7 +3646,7 @@
         <v>0</v>
       </c>
       <c r="J82" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K82" s="7" t="b">
         <v>1</v>
@@ -3660,31 +3657,31 @@
         <v>95</v>
       </c>
       <c r="B83" s="5">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C83" s="5">
+        <v>26</v>
+      </c>
+      <c r="D83" s="5">
+        <v>12</v>
+      </c>
+      <c r="E83" s="5">
         <v>30</v>
-      </c>
-      <c r="D83" s="5">
-        <v>16</v>
-      </c>
-      <c r="E83" s="5">
-        <v>34</v>
       </c>
       <c r="F83" s="5">
         <v>5</v>
       </c>
       <c r="G83" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H83" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I83" s="5" t="b">
         <v>0</v>
       </c>
       <c r="J83" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K83" s="7" t="b">
         <v>1</v>
@@ -3719,7 +3716,7 @@
         <v>0</v>
       </c>
       <c r="J84" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K84" s="7" t="b">
         <v>1</v>
@@ -3730,22 +3727,22 @@
         <v>97</v>
       </c>
       <c r="B85" s="5">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C85" s="5">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="D85" s="5">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E85" s="5">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F85" s="5">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G85" s="5">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="H85" s="5" t="b">
         <v>0</v>
@@ -3754,7 +3751,7 @@
         <v>0</v>
       </c>
       <c r="J85" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K85" s="7" t="b">
         <v>1</v>
@@ -3765,31 +3762,31 @@
         <v>98</v>
       </c>
       <c r="B86" s="5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C86" s="5">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="D86" s="5">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E86" s="5">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="F86" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G86" s="5">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="H86" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I86" s="5" t="b">
         <v>0</v>
       </c>
       <c r="J86" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K86" s="7" t="b">
         <v>1</v>
@@ -3800,31 +3797,31 @@
         <v>99</v>
       </c>
       <c r="B87" s="5">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C87" s="5">
+        <v>24</v>
+      </c>
+      <c r="D87" s="5">
+        <v>10</v>
+      </c>
+      <c r="E87" s="5">
         <v>28</v>
       </c>
-      <c r="D87" s="5">
-        <v>16</v>
-      </c>
-      <c r="E87" s="5">
+      <c r="F87" s="5">
+        <v>2</v>
+      </c>
+      <c r="G87" s="5">
         <v>32</v>
       </c>
-      <c r="F87" s="5">
-        <v>10</v>
-      </c>
-      <c r="G87" s="5">
-        <v>36</v>
-      </c>
       <c r="H87" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I87" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J87" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K87" s="7" t="b">
         <v>1</v>
@@ -3835,22 +3832,22 @@
         <v>100</v>
       </c>
       <c r="B88" s="5">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C88" s="5">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D88" s="5">
+        <v>18</v>
+      </c>
+      <c r="E88" s="5">
+        <v>30</v>
+      </c>
+      <c r="F88" s="5">
         <v>10</v>
       </c>
-      <c r="E88" s="5">
-        <v>28</v>
-      </c>
-      <c r="F88" s="5">
-        <v>2</v>
-      </c>
       <c r="G88" s="5">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H88" s="5" t="b">
         <v>1</v>
@@ -3859,7 +3856,7 @@
         <v>1</v>
       </c>
       <c r="J88" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K88" s="7" t="b">
         <v>1</v>
@@ -3870,23 +3867,23 @@
         <v>101</v>
       </c>
       <c r="B89" s="5">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C89" s="5">
+        <v>20</v>
+      </c>
+      <c r="D89" s="5">
+        <v>5</v>
+      </c>
+      <c r="E89" s="5">
+        <v>24</v>
+      </c>
+      <c r="F89" s="5">
+        <v>0</v>
+      </c>
+      <c r="G89" s="5">
         <v>28</v>
       </c>
-      <c r="D89" s="5">
-        <v>18</v>
-      </c>
-      <c r="E89" s="5">
-        <v>30</v>
-      </c>
-      <c r="F89" s="5">
-        <v>10</v>
-      </c>
-      <c r="G89" s="5">
-        <v>34</v>
-      </c>
       <c r="H89" s="5" t="b">
         <v>1</v>
       </c>
@@ -3894,7 +3891,7 @@
         <v>1</v>
       </c>
       <c r="J89" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K89" s="7" t="b">
         <v>1</v>
@@ -3929,7 +3926,7 @@
         <v>1</v>
       </c>
       <c r="J90" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K90" s="7" t="b">
         <v>1</v>
@@ -3940,22 +3937,22 @@
         <v>103</v>
       </c>
       <c r="B91" s="5">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C91" s="5">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D91" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E91" s="5">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F91" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G91" s="5">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H91" s="5" t="b">
         <v>1</v>
@@ -3964,7 +3961,7 @@
         <v>1</v>
       </c>
       <c r="J91" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K91" s="7" t="b">
         <v>1</v>
@@ -3975,31 +3972,31 @@
         <v>104</v>
       </c>
       <c r="B92" s="5">
+        <v>22</v>
+      </c>
+      <c r="C92" s="5">
+        <v>30</v>
+      </c>
+      <c r="D92" s="5">
         <v>16</v>
       </c>
-      <c r="C92" s="5">
-        <v>24</v>
-      </c>
-      <c r="D92" s="5">
-        <v>10</v>
-      </c>
       <c r="E92" s="5">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F92" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G92" s="5">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H92" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I92" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J92" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K92" s="7" t="b">
         <v>1</v>
@@ -4010,31 +4007,31 @@
         <v>105</v>
       </c>
       <c r="B93" s="5">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C93" s="5">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D93" s="5">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E93" s="5">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F93" s="5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G93" s="5">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H93" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I93" s="5" t="b">
         <v>0</v>
       </c>
       <c r="J93" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K93" s="7" t="b">
         <v>1</v>
@@ -4045,31 +4042,31 @@
         <v>106</v>
       </c>
       <c r="B94" s="5">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C94" s="5">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D94" s="5">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E94" s="5">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F94" s="5">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="G94" s="5">
-        <v>35</v>
-      </c>
-      <c r="H94" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I94" s="5" t="b">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="H94" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I94" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="J94" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K94" s="7" t="b">
         <v>1</v>
@@ -4104,44 +4101,9 @@
         <v>1</v>
       </c>
       <c r="J95" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K95" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11">
-      <c r="A96" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B96" s="5">
-        <v>14</v>
-      </c>
-      <c r="C96" s="5">
-        <v>22</v>
-      </c>
-      <c r="D96" s="5">
-        <v>6</v>
-      </c>
-      <c r="E96" s="5">
-        <v>26</v>
-      </c>
-      <c r="F96" s="5">
-        <v>-20</v>
-      </c>
-      <c r="G96" s="5">
-        <v>30</v>
-      </c>
-      <c r="H96" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I96" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J96" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K96" s="7" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Light requirement & some state transition flags
</commit_message>
<xml_diff>
--- a/src/datagen/resources/data/frostedheart/data/plant_temperature.xlsx
+++ b/src/datagen/resources/data/frostedheart/data/plant_temperature.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyc/Development/FrostedHeart/src/datagen/resources/data/frostedheart/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D626A15-8213-F346-8510-BAE1AE9D57F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CB9753-D855-0F47-8681-E6F1FDA74C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="116">
   <si>
     <t>block</t>
   </si>
@@ -361,6 +361,15 @@
   </si>
   <si>
     <t>supplementaries:wild_flax</t>
+  </si>
+  <si>
+    <t>heat_capacity</t>
+  </si>
+  <si>
+    <t>min_skylight</t>
+  </si>
+  <si>
+    <t>max_skylight</t>
   </si>
 </sst>
 </file>
@@ -775,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L98"/>
+  <dimension ref="A1:O98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="N64" sqref="N64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -795,9 +804,12 @@
     <col min="10" max="10" width="13.33203125" style="5" customWidth="1"/>
     <col min="11" max="11" width="28.33203125" customWidth="1"/>
     <col min="12" max="12" width="11.6640625" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" customWidth="1"/>
+    <col min="14" max="14" width="13.1640625" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="23.25" customHeight="1">
+    <row r="1" spans="1:15" ht="23.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -834,8 +846,17 @@
       <c r="L1" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1">
+      <c r="M1" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="14.25" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -872,8 +893,17 @@
       <c r="L2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="14.25" customHeight="1">
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -910,8 +940,17 @@
       <c r="L3" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3">
+        <v>10</v>
+      </c>
+      <c r="N3">
+        <v>9</v>
+      </c>
+      <c r="O3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -948,8 +987,17 @@
       <c r="L4" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4">
+        <v>10</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -986,8 +1034,17 @@
       <c r="L5" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5">
+        <v>10</v>
+      </c>
+      <c r="N5">
+        <v>9</v>
+      </c>
+      <c r="O5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
@@ -1024,8 +1081,17 @@
       <c r="L6" s="8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6">
+        <v>10</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
@@ -1062,8 +1128,17 @@
       <c r="L7" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7">
+        <v>10</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -1100,8 +1175,17 @@
       <c r="L8" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8">
+        <v>10</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -1138,8 +1222,17 @@
       <c r="L9" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9">
+        <v>10</v>
+      </c>
+      <c r="N9">
+        <v>14</v>
+      </c>
+      <c r="O9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
@@ -1176,8 +1269,17 @@
       <c r="L10" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10">
+        <v>10</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
@@ -1214,8 +1316,17 @@
       <c r="L11" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11">
+        <v>10</v>
+      </c>
+      <c r="N11">
+        <v>14</v>
+      </c>
+      <c r="O11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
@@ -1252,8 +1363,17 @@
       <c r="L12" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12">
+        <v>10</v>
+      </c>
+      <c r="N12">
+        <v>14</v>
+      </c>
+      <c r="O12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="5" t="s">
         <v>28</v>
       </c>
@@ -1290,8 +1410,17 @@
       <c r="L13" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13">
+        <v>10</v>
+      </c>
+      <c r="N13">
+        <v>14</v>
+      </c>
+      <c r="O13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="5" t="s">
         <v>29</v>
       </c>
@@ -1328,8 +1457,17 @@
       <c r="L14" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14">
+        <v>10</v>
+      </c>
+      <c r="N14">
+        <v>14</v>
+      </c>
+      <c r="O14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="5" t="s">
         <v>30</v>
       </c>
@@ -1366,8 +1504,17 @@
       <c r="L15" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15">
+        <v>10</v>
+      </c>
+      <c r="N15">
+        <v>14</v>
+      </c>
+      <c r="O15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
@@ -1404,8 +1551,17 @@
       <c r="L16" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16">
+        <v>10</v>
+      </c>
+      <c r="N16">
+        <v>14</v>
+      </c>
+      <c r="O16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
@@ -1442,8 +1598,17 @@
       <c r="L17" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17">
+        <v>10</v>
+      </c>
+      <c r="N17">
+        <v>14</v>
+      </c>
+      <c r="O17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="5" t="s">
         <v>33</v>
       </c>
@@ -1480,8 +1645,17 @@
       <c r="L18" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18">
+        <v>10</v>
+      </c>
+      <c r="N18">
+        <v>14</v>
+      </c>
+      <c r="O18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="5" t="s">
         <v>34</v>
       </c>
@@ -1518,8 +1692,17 @@
       <c r="L19" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19">
+        <v>10</v>
+      </c>
+      <c r="N19">
+        <v>14</v>
+      </c>
+      <c r="O19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="5" t="s">
         <v>35</v>
       </c>
@@ -1556,8 +1739,17 @@
       <c r="L20" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="M20">
+        <v>10</v>
+      </c>
+      <c r="N20">
+        <v>14</v>
+      </c>
+      <c r="O20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="5" t="s">
         <v>36</v>
       </c>
@@ -1594,8 +1786,17 @@
       <c r="L21" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21">
+        <v>10</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="5" t="s">
         <v>37</v>
       </c>
@@ -1632,8 +1833,17 @@
       <c r="L22" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22">
+        <v>10</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="4" t="s">
         <v>38</v>
       </c>
@@ -1670,8 +1880,17 @@
       <c r="L23" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="M23">
+        <v>10</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="4" t="s">
         <v>39</v>
       </c>
@@ -1708,8 +1927,17 @@
       <c r="L24" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24">
+        <v>10</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="5" t="s">
         <v>40</v>
       </c>
@@ -1746,8 +1974,17 @@
       <c r="L25" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25">
+        <v>10</v>
+      </c>
+      <c r="N25">
+        <v>9</v>
+      </c>
+      <c r="O25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="5" t="s">
         <v>41</v>
       </c>
@@ -1784,8 +2021,17 @@
       <c r="L26" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="M26">
+        <v>10</v>
+      </c>
+      <c r="N26">
+        <v>9</v>
+      </c>
+      <c r="O26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="5" t="s">
         <v>42</v>
       </c>
@@ -1822,8 +2068,17 @@
       <c r="L27" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="M27">
+        <v>10</v>
+      </c>
+      <c r="N27">
+        <v>9</v>
+      </c>
+      <c r="O27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" s="5" t="s">
         <v>43</v>
       </c>
@@ -1860,8 +2115,17 @@
       <c r="L28" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="M28">
+        <v>10</v>
+      </c>
+      <c r="N28">
+        <v>9</v>
+      </c>
+      <c r="O28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" s="5" t="s">
         <v>44</v>
       </c>
@@ -1898,8 +2162,17 @@
       <c r="L29" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="M29">
+        <v>10</v>
+      </c>
+      <c r="N29">
+        <v>9</v>
+      </c>
+      <c r="O29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" s="5" t="s">
         <v>45</v>
       </c>
@@ -1936,8 +2209,17 @@
       <c r="L30" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="M30">
+        <v>10</v>
+      </c>
+      <c r="N30">
+        <v>9</v>
+      </c>
+      <c r="O30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" s="5" t="s">
         <v>46</v>
       </c>
@@ -1974,8 +2256,17 @@
       <c r="L31" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="M31">
+        <v>10</v>
+      </c>
+      <c r="N31">
+        <v>9</v>
+      </c>
+      <c r="O31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" s="5" t="s">
         <v>47</v>
       </c>
@@ -2012,8 +2303,17 @@
       <c r="L32" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="M32">
+        <v>10</v>
+      </c>
+      <c r="N32">
+        <v>9</v>
+      </c>
+      <c r="O32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" s="5" t="s">
         <v>48</v>
       </c>
@@ -2050,8 +2350,17 @@
       <c r="L33" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="M33">
+        <v>10</v>
+      </c>
+      <c r="N33">
+        <v>9</v>
+      </c>
+      <c r="O33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="5" t="s">
         <v>49</v>
       </c>
@@ -2088,8 +2397,17 @@
       <c r="L34" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="M34">
+        <v>10</v>
+      </c>
+      <c r="N34">
+        <v>9</v>
+      </c>
+      <c r="O34">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" s="5" t="s">
         <v>50</v>
       </c>
@@ -2126,8 +2444,17 @@
       <c r="L35" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="M35">
+        <v>10</v>
+      </c>
+      <c r="N35">
+        <v>9</v>
+      </c>
+      <c r="O35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" s="5" t="s">
         <v>51</v>
       </c>
@@ -2164,8 +2491,17 @@
       <c r="L36" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="M36">
+        <v>10</v>
+      </c>
+      <c r="N36">
+        <v>9</v>
+      </c>
+      <c r="O36">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" s="5" t="s">
         <v>52</v>
       </c>
@@ -2202,8 +2538,17 @@
       <c r="L37" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="M37">
+        <v>10</v>
+      </c>
+      <c r="N37">
+        <v>9</v>
+      </c>
+      <c r="O37">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" s="5" t="s">
         <v>53</v>
       </c>
@@ -2240,8 +2585,17 @@
       <c r="L38" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="M38">
+        <v>10</v>
+      </c>
+      <c r="N38">
+        <v>9</v>
+      </c>
+      <c r="O38">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" s="5" t="s">
         <v>54</v>
       </c>
@@ -2278,8 +2632,17 @@
       <c r="L39" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="M39">
+        <v>10</v>
+      </c>
+      <c r="N39">
+        <v>9</v>
+      </c>
+      <c r="O39">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" s="5" t="s">
         <v>55</v>
       </c>
@@ -2316,8 +2679,17 @@
       <c r="L40" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:12">
+      <c r="M40">
+        <v>10</v>
+      </c>
+      <c r="N40">
+        <v>9</v>
+      </c>
+      <c r="O40">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" s="5" t="s">
         <v>56</v>
       </c>
@@ -2354,8 +2726,17 @@
       <c r="L41" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:12">
+      <c r="M41">
+        <v>10</v>
+      </c>
+      <c r="N41">
+        <v>9</v>
+      </c>
+      <c r="O41">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" s="5" t="s">
         <v>57</v>
       </c>
@@ -2392,8 +2773,17 @@
       <c r="L42" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="M42">
+        <v>10</v>
+      </c>
+      <c r="N42">
+        <v>12</v>
+      </c>
+      <c r="O42">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43" s="5" t="s">
         <v>58</v>
       </c>
@@ -2430,8 +2820,17 @@
       <c r="L43" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:12">
+      <c r="M43">
+        <v>10</v>
+      </c>
+      <c r="N43">
+        <v>12</v>
+      </c>
+      <c r="O43">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" s="5" t="s">
         <v>59</v>
       </c>
@@ -2468,8 +2867,17 @@
       <c r="L44" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:12">
+      <c r="M44">
+        <v>10</v>
+      </c>
+      <c r="N44">
+        <v>12</v>
+      </c>
+      <c r="O44">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45" s="4" t="s">
         <v>60</v>
       </c>
@@ -2506,8 +2914,17 @@
       <c r="L45" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="M45">
+        <v>10</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46" s="4" t="s">
         <v>61</v>
       </c>
@@ -2544,8 +2961,17 @@
       <c r="L46" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="M46">
+        <v>10</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47" s="9" t="s">
         <v>62</v>
       </c>
@@ -2582,8 +3008,17 @@
       <c r="L47" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:12">
+      <c r="M47">
+        <v>10</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48" s="9" t="s">
         <v>63</v>
       </c>
@@ -2620,8 +3055,17 @@
       <c r="L48" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:12">
+      <c r="M48">
+        <v>10</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49" s="9" t="s">
         <v>64</v>
       </c>
@@ -2658,8 +3102,17 @@
       <c r="L49" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:12">
+      <c r="M49">
+        <v>10</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" s="5" t="s">
         <v>108</v>
       </c>
@@ -2696,8 +3149,17 @@
       <c r="L50" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:12">
+      <c r="M50">
+        <v>10</v>
+      </c>
+      <c r="N50">
+        <v>9</v>
+      </c>
+      <c r="O50">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51" s="5" t="s">
         <v>65</v>
       </c>
@@ -2734,8 +3196,17 @@
       <c r="L51" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="M51">
+        <v>10</v>
+      </c>
+      <c r="N51">
+        <v>9</v>
+      </c>
+      <c r="O51">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
       <c r="A52" s="5" t="s">
         <v>66</v>
       </c>
@@ -2772,8 +3243,17 @@
       <c r="L52" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:12">
+      <c r="M52">
+        <v>10</v>
+      </c>
+      <c r="N52">
+        <v>9</v>
+      </c>
+      <c r="O52">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
       <c r="A53" s="5" t="s">
         <v>67</v>
       </c>
@@ -2810,8 +3290,17 @@
       <c r="L53" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:12">
+      <c r="M53">
+        <v>10</v>
+      </c>
+      <c r="N53">
+        <v>9</v>
+      </c>
+      <c r="O53">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
       <c r="A54" s="5" t="s">
         <v>68</v>
       </c>
@@ -2848,8 +3337,17 @@
       <c r="L54" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:12">
+      <c r="M54">
+        <v>10</v>
+      </c>
+      <c r="N54">
+        <v>9</v>
+      </c>
+      <c r="O54">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
       <c r="A55" s="5" t="s">
         <v>69</v>
       </c>
@@ -2886,8 +3384,17 @@
       <c r="L55" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:12">
+      <c r="M55">
+        <v>10</v>
+      </c>
+      <c r="N55">
+        <v>9</v>
+      </c>
+      <c r="O55">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
       <c r="A56" s="5" t="s">
         <v>70</v>
       </c>
@@ -2924,8 +3431,17 @@
       <c r="L56" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="M56">
+        <v>10</v>
+      </c>
+      <c r="N56">
+        <v>9</v>
+      </c>
+      <c r="O56">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
       <c r="A57" s="5" t="s">
         <v>71</v>
       </c>
@@ -2962,8 +3478,17 @@
       <c r="L57" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:12">
+      <c r="M57">
+        <v>10</v>
+      </c>
+      <c r="N57">
+        <v>9</v>
+      </c>
+      <c r="O57">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
       <c r="A58" s="5" t="s">
         <v>72</v>
       </c>
@@ -3000,8 +3525,17 @@
       <c r="L58" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:12">
+      <c r="M58">
+        <v>10</v>
+      </c>
+      <c r="N58">
+        <v>9</v>
+      </c>
+      <c r="O58">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59" s="5" t="s">
         <v>73</v>
       </c>
@@ -3038,8 +3572,17 @@
       <c r="L59" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:12">
+      <c r="M59">
+        <v>10</v>
+      </c>
+      <c r="N59">
+        <v>9</v>
+      </c>
+      <c r="O59">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60" s="5" t="s">
         <v>74</v>
       </c>
@@ -3076,8 +3619,17 @@
       <c r="L60" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:12">
+      <c r="M60">
+        <v>100</v>
+      </c>
+      <c r="N60">
+        <v>9</v>
+      </c>
+      <c r="O60">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
       <c r="A61" s="5" t="s">
         <v>11</v>
       </c>
@@ -3114,8 +3666,17 @@
       <c r="L61" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:12">
+      <c r="M61">
+        <v>10</v>
+      </c>
+      <c r="N61">
+        <v>12</v>
+      </c>
+      <c r="O61">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
       <c r="A62" s="5" t="s">
         <v>75</v>
       </c>
@@ -3152,8 +3713,17 @@
       <c r="L62" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:12">
+      <c r="M62">
+        <v>10</v>
+      </c>
+      <c r="N62">
+        <v>9</v>
+      </c>
+      <c r="O62">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
       <c r="A63" s="5" t="s">
         <v>76</v>
       </c>
@@ -3190,8 +3760,17 @@
       <c r="L63" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:12">
+      <c r="M63">
+        <v>10</v>
+      </c>
+      <c r="N63">
+        <v>12</v>
+      </c>
+      <c r="O63">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
       <c r="A64" s="5" t="s">
         <v>77</v>
       </c>
@@ -3228,8 +3807,17 @@
       <c r="L64" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:12">
+      <c r="M64">
+        <v>10</v>
+      </c>
+      <c r="N64">
+        <v>12</v>
+      </c>
+      <c r="O64">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
       <c r="A65" s="5" t="s">
         <v>78</v>
       </c>
@@ -3266,8 +3854,17 @@
       <c r="L65" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:12">
+      <c r="M65">
+        <v>10</v>
+      </c>
+      <c r="N65">
+        <v>9</v>
+      </c>
+      <c r="O65">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
       <c r="A66" s="5" t="s">
         <v>79</v>
       </c>
@@ -3304,8 +3901,17 @@
       <c r="L66" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:12">
+      <c r="M66">
+        <v>10</v>
+      </c>
+      <c r="N66">
+        <v>9</v>
+      </c>
+      <c r="O66">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15">
       <c r="A67" s="5" t="s">
         <v>80</v>
       </c>
@@ -3342,8 +3948,17 @@
       <c r="L67" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:12">
+      <c r="M67">
+        <v>10</v>
+      </c>
+      <c r="N67">
+        <v>12</v>
+      </c>
+      <c r="O67">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15">
       <c r="A68" s="5" t="s">
         <v>81</v>
       </c>
@@ -3380,8 +3995,17 @@
       <c r="L68" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:12">
+      <c r="M68">
+        <v>10</v>
+      </c>
+      <c r="N68">
+        <v>9</v>
+      </c>
+      <c r="O68">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
       <c r="A69" s="5" t="s">
         <v>82</v>
       </c>
@@ -3418,8 +4042,17 @@
       <c r="L69" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:12">
+      <c r="M69">
+        <v>10</v>
+      </c>
+      <c r="N69">
+        <v>9</v>
+      </c>
+      <c r="O69">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15">
       <c r="A70" s="5" t="s">
         <v>9</v>
       </c>
@@ -3456,8 +4089,17 @@
       <c r="L70" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:12">
+      <c r="M70">
+        <v>10</v>
+      </c>
+      <c r="N70">
+        <v>9</v>
+      </c>
+      <c r="O70">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15">
       <c r="A71" s="5" t="s">
         <v>83</v>
       </c>
@@ -3494,8 +4136,17 @@
       <c r="L71" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:12">
+      <c r="M71">
+        <v>10</v>
+      </c>
+      <c r="N71">
+        <v>12</v>
+      </c>
+      <c r="O71">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15">
       <c r="A72" s="5" t="s">
         <v>84</v>
       </c>
@@ -3532,8 +4183,17 @@
       <c r="L72" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:12">
+      <c r="M72">
+        <v>10</v>
+      </c>
+      <c r="N72">
+        <v>0</v>
+      </c>
+      <c r="O72">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15">
       <c r="A73" s="5" t="s">
         <v>85</v>
       </c>
@@ -3570,8 +4230,17 @@
       <c r="L73" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:12">
+      <c r="M73">
+        <v>10</v>
+      </c>
+      <c r="N73">
+        <v>0</v>
+      </c>
+      <c r="O73">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15">
       <c r="A74" s="5" t="s">
         <v>86</v>
       </c>
@@ -3608,8 +4277,17 @@
       <c r="L74" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:12">
+      <c r="M74">
+        <v>10</v>
+      </c>
+      <c r="N74">
+        <v>14</v>
+      </c>
+      <c r="O74">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15">
       <c r="A75" s="5" t="s">
         <v>87</v>
       </c>
@@ -3646,8 +4324,17 @@
       <c r="L75" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:12">
+      <c r="M75">
+        <v>10</v>
+      </c>
+      <c r="N75">
+        <v>14</v>
+      </c>
+      <c r="O75">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15">
       <c r="A76" s="5" t="s">
         <v>88</v>
       </c>
@@ -3684,8 +4371,17 @@
       <c r="L76" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:12">
+      <c r="M76">
+        <v>10</v>
+      </c>
+      <c r="N76">
+        <v>14</v>
+      </c>
+      <c r="O76">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15">
       <c r="A77" s="5" t="s">
         <v>89</v>
       </c>
@@ -3722,8 +4418,17 @@
       <c r="L77" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:12">
+      <c r="M77">
+        <v>10</v>
+      </c>
+      <c r="N77">
+        <v>14</v>
+      </c>
+      <c r="O77">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15">
       <c r="A78" s="5" t="s">
         <v>90</v>
       </c>
@@ -3760,8 +4465,17 @@
       <c r="L78" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:12">
+      <c r="M78">
+        <v>10</v>
+      </c>
+      <c r="N78">
+        <v>14</v>
+      </c>
+      <c r="O78">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15">
       <c r="A79" s="5" t="s">
         <v>91</v>
       </c>
@@ -3798,8 +4512,17 @@
       <c r="L79" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:12">
+      <c r="M79">
+        <v>10</v>
+      </c>
+      <c r="N79">
+        <v>14</v>
+      </c>
+      <c r="O79">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15">
       <c r="A80" s="5" t="s">
         <v>92</v>
       </c>
@@ -3836,8 +4559,17 @@
       <c r="L80" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:12">
+      <c r="M80">
+        <v>10</v>
+      </c>
+      <c r="N80">
+        <v>14</v>
+      </c>
+      <c r="O80">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15">
       <c r="A81" s="5" t="s">
         <v>93</v>
       </c>
@@ -3874,8 +4606,17 @@
       <c r="L81" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:12">
+      <c r="M81">
+        <v>10</v>
+      </c>
+      <c r="N81">
+        <v>14</v>
+      </c>
+      <c r="O81">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15">
       <c r="A82" s="5" t="s">
         <v>94</v>
       </c>
@@ -3912,8 +4653,17 @@
       <c r="L82" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:12">
+      <c r="M82">
+        <v>10</v>
+      </c>
+      <c r="N82">
+        <v>14</v>
+      </c>
+      <c r="O82">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15">
       <c r="A83" s="5" t="s">
         <v>95</v>
       </c>
@@ -3950,8 +4700,17 @@
       <c r="L83" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:12">
+      <c r="M83">
+        <v>10</v>
+      </c>
+      <c r="N83">
+        <v>0</v>
+      </c>
+      <c r="O83">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15">
       <c r="A84" s="5" t="s">
         <v>96</v>
       </c>
@@ -3988,8 +4747,17 @@
       <c r="L84" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:12">
+      <c r="M84">
+        <v>10</v>
+      </c>
+      <c r="N84">
+        <v>0</v>
+      </c>
+      <c r="O84">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15">
       <c r="A85" s="5" t="s">
         <v>97</v>
       </c>
@@ -4026,8 +4794,17 @@
       <c r="L85" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:12">
+      <c r="M85">
+        <v>10</v>
+      </c>
+      <c r="N85">
+        <v>0</v>
+      </c>
+      <c r="O85">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15">
       <c r="A86" s="5" t="s">
         <v>98</v>
       </c>
@@ -4064,8 +4841,17 @@
       <c r="L86" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:12">
+      <c r="M86">
+        <v>10</v>
+      </c>
+      <c r="N86">
+        <v>6</v>
+      </c>
+      <c r="O86">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15">
       <c r="A87" s="5" t="s">
         <v>99</v>
       </c>
@@ -4102,8 +4888,17 @@
       <c r="L87" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:12">
+      <c r="M87">
+        <v>10</v>
+      </c>
+      <c r="N87">
+        <v>6</v>
+      </c>
+      <c r="O87">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15">
       <c r="A88" s="5" t="s">
         <v>100</v>
       </c>
@@ -4140,8 +4935,17 @@
       <c r="L88" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:12">
+      <c r="M88">
+        <v>10</v>
+      </c>
+      <c r="N88">
+        <v>6</v>
+      </c>
+      <c r="O88">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15">
       <c r="A89" s="5" t="s">
         <v>101</v>
       </c>
@@ -4178,8 +4982,17 @@
       <c r="L89" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:12">
+      <c r="M89">
+        <v>10</v>
+      </c>
+      <c r="N89">
+        <v>6</v>
+      </c>
+      <c r="O89">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15">
       <c r="A90" s="5" t="s">
         <v>102</v>
       </c>
@@ -4216,8 +5029,17 @@
       <c r="L90" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:12">
+      <c r="M90">
+        <v>10</v>
+      </c>
+      <c r="N90">
+        <v>6</v>
+      </c>
+      <c r="O90">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15">
       <c r="A91" s="5" t="s">
         <v>103</v>
       </c>
@@ -4254,8 +5076,17 @@
       <c r="L91" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:12">
+      <c r="M91">
+        <v>10</v>
+      </c>
+      <c r="N91">
+        <v>6</v>
+      </c>
+      <c r="O91">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15">
       <c r="A92" s="5" t="s">
         <v>104</v>
       </c>
@@ -4292,8 +5123,17 @@
       <c r="L92" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:12">
+      <c r="M92">
+        <v>10</v>
+      </c>
+      <c r="N92">
+        <v>12</v>
+      </c>
+      <c r="O92">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15">
       <c r="A93" s="5" t="s">
         <v>105</v>
       </c>
@@ -4330,8 +5170,17 @@
       <c r="L93" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:12">
+      <c r="M93">
+        <v>10</v>
+      </c>
+      <c r="N93">
+        <v>12</v>
+      </c>
+      <c r="O93">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15">
       <c r="A94" s="5" t="s">
         <v>106</v>
       </c>
@@ -4368,8 +5217,17 @@
       <c r="L94" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:12">
+      <c r="M94">
+        <v>10</v>
+      </c>
+      <c r="N94">
+        <v>9</v>
+      </c>
+      <c r="O94">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15">
       <c r="A95" s="5" t="s">
         <v>107</v>
       </c>
@@ -4406,8 +5264,17 @@
       <c r="L95" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:12">
+      <c r="M95">
+        <v>10</v>
+      </c>
+      <c r="N95">
+        <v>9</v>
+      </c>
+      <c r="O95">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15">
       <c r="A96" s="5" t="s">
         <v>110</v>
       </c>
@@ -4444,8 +5311,17 @@
       <c r="L96" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:12">
+      <c r="M96">
+        <v>10</v>
+      </c>
+      <c r="N96">
+        <v>12</v>
+      </c>
+      <c r="O96">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15">
       <c r="A97" s="5" t="s">
         <v>111</v>
       </c>
@@ -4482,8 +5358,17 @@
       <c r="L97" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:12">
+      <c r="M97">
+        <v>10</v>
+      </c>
+      <c r="N97">
+        <v>12</v>
+      </c>
+      <c r="O97">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15">
       <c r="A98" s="5" t="s">
         <v>112</v>
       </c>
@@ -4519,6 +5404,15 @@
       </c>
       <c r="L98" s="7" t="b">
         <v>1</v>
+      </c>
+      <c r="M98">
+        <v>10</v>
+      </c>
+      <c r="N98">
+        <v>12</v>
+      </c>
+      <c r="O98">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fully fixed state trans
</commit_message>
<xml_diff>
--- a/src/datagen/resources/data/frostedheart/data/plant_temperature.xlsx
+++ b/src/datagen/resources/data/frostedheart/data/plant_temperature.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyc/Development/FrostedHeart/src/datagen/resources/data/frostedheart/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\eclipse-workspace\frostedheart-newdev\src\datagen\resources\data\frostedheart\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBFE690-EF36-D543-828B-340CDDF0540D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5741EEA-1DF8-4C2A-BEBD-438ECA8DA69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="34995" windowHeight="19060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="118">
   <si>
     <t>block</t>
   </si>
@@ -370,6 +370,14 @@
   </si>
   <si>
     <t>max_skylight</t>
+  </si>
+  <si>
+    <t>minecraft:dead_bush</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>minecraft:dirt</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -472,7 +480,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -786,30 +794,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="L60" sqref="L60"/>
+    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.3"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="23.625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="5" customWidth="1"/>
     <col min="4" max="4" width="12" style="5" customWidth="1"/>
     <col min="5" max="5" width="9" style="5"/>
-    <col min="6" max="6" width="9.1640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="9.125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="11.875" style="5" customWidth="1"/>
     <col min="9" max="9" width="12.5" style="5" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="28.33203125" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" customWidth="1"/>
-    <col min="14" max="14" width="13.1640625" customWidth="1"/>
+    <col min="10" max="10" width="13.375" style="5" customWidth="1"/>
+    <col min="11" max="11" width="28.375" customWidth="1"/>
+    <col min="12" max="12" width="11.625" customWidth="1"/>
+    <col min="13" max="13" width="13.875" customWidth="1"/>
+    <col min="14" max="14" width="13.125" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="23.25" customHeight="1">
+    <row r="1" spans="1:15" ht="23.3" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -856,7 +864,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="14.25" customHeight="1">
+    <row r="2" spans="1:15" ht="14.3" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -903,7 +911,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="14.25" customHeight="1">
+    <row r="3" spans="1:15" ht="14.3" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -935,7 +943,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
       <c r="L3" s="7" t="b">
         <v>1</v>
@@ -1029,7 +1037,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
       <c r="L5" s="7" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Night Soil Collector and some misc fix on trade
</commit_message>
<xml_diff>
--- a/src/datagen/resources/data/frostedheart/data/plant_temperature.xlsx
+++ b/src/datagen/resources/data/frostedheart/data/plant_temperature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyc/Development/FrostedHeart/src/datagen/resources/data/frostedheart/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBCDDF1-9C72-DF4A-A0E9-2B85B1D69E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F68B94-6FE6-BC4B-9A24-BD2F3F88DE25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -456,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -470,6 +470,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="L84" sqref="L84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1957,7 +1958,7 @@
         <v>32</v>
       </c>
       <c r="G25" s="5">
-        <v>-10</v>
+        <v>-40</v>
       </c>
       <c r="H25" s="5">
         <v>40</v>
@@ -2004,7 +2005,7 @@
         <v>28</v>
       </c>
       <c r="G26" s="5">
-        <v>-5</v>
+        <v>-40</v>
       </c>
       <c r="H26" s="5">
         <v>35</v>
@@ -2098,7 +2099,7 @@
         <v>28</v>
       </c>
       <c r="G28" s="5">
-        <v>-5</v>
+        <v>-40</v>
       </c>
       <c r="H28" s="5">
         <v>35</v>
@@ -3179,7 +3180,7 @@
         <v>32</v>
       </c>
       <c r="G51" s="5">
-        <v>-10</v>
+        <v>-40</v>
       </c>
       <c r="H51" s="5">
         <v>40</v>
@@ -4682,8 +4683,8 @@
       <c r="F83" s="5">
         <v>30</v>
       </c>
-      <c r="G83" s="5">
-        <v>5</v>
+      <c r="G83" s="13">
+        <v>-40</v>
       </c>
       <c r="H83" s="5">
         <v>35</v>
@@ -4729,8 +4730,8 @@
       <c r="F84" s="5">
         <v>30</v>
       </c>
-      <c r="G84" s="5">
-        <v>5</v>
+      <c r="G84" s="13">
+        <v>-40</v>
       </c>
       <c r="H84" s="5">
         <v>35</v>
@@ -4886,7 +4887,7 @@
         <v>22</v>
       </c>
       <c r="L87" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M87">
         <v>10</v>
@@ -4933,7 +4934,7 @@
         <v>22</v>
       </c>
       <c r="L88" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M88">
         <v>10</v>
@@ -4980,7 +4981,7 @@
         <v>22</v>
       </c>
       <c r="L89" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M89">
         <v>10</v>
@@ -5027,7 +5028,7 @@
         <v>22</v>
       </c>
       <c r="L90" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M90">
         <v>10</v>
@@ -5074,7 +5075,7 @@
         <v>22</v>
       </c>
       <c r="L91" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M91">
         <v>10</v>

</xml_diff>

<commit_message>
Reduce some light requirements
</commit_message>
<xml_diff>
--- a/src/datagen/resources/data/frostedheart/data/plant_temperature.xlsx
+++ b/src/datagen/resources/data/frostedheart/data/plant_temperature.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyc/Development/FrostedHeart/src/datagen/resources/data/frostedheart/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F68B94-6FE6-BC4B-9A24-BD2F3F88DE25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549095F9-C8F3-1745-914A-374097FA7BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34500" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -456,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -470,7 +470,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="L84" sqref="L84"/>
+    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1227,7 +1226,7 @@
         <v>10</v>
       </c>
       <c r="N9">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="O9">
         <v>15</v>
@@ -1661,7 +1660,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="12">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C19" s="5">
         <v>14</v>
@@ -1697,7 +1696,7 @@
         <v>10</v>
       </c>
       <c r="N19">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="O19">
         <v>15</v>
@@ -1708,7 +1707,7 @@
         <v>35</v>
       </c>
       <c r="B20" s="12">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C20" s="5">
         <v>14</v>
@@ -1744,7 +1743,7 @@
         <v>10</v>
       </c>
       <c r="N20">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="O20">
         <v>15</v>
@@ -3718,7 +3717,7 @@
         <v>10</v>
       </c>
       <c r="N62">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="O62">
         <v>15</v>
@@ -4329,7 +4328,7 @@
         <v>10</v>
       </c>
       <c r="N75">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="O75">
         <v>15</v>
@@ -4376,7 +4375,7 @@
         <v>10</v>
       </c>
       <c r="N76">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="O76">
         <v>15</v>
@@ -4470,7 +4469,7 @@
         <v>10</v>
       </c>
       <c r="N78">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="O78">
         <v>15</v>
@@ -4517,7 +4516,7 @@
         <v>10</v>
       </c>
       <c r="N79">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="O79">
         <v>15</v>
@@ -4611,7 +4610,7 @@
         <v>10</v>
       </c>
       <c r="N81">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="O81">
         <v>15</v>
@@ -4658,7 +4657,7 @@
         <v>10</v>
       </c>
       <c r="N82">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="O82">
         <v>15</v>
@@ -4683,7 +4682,7 @@
       <c r="F83" s="5">
         <v>30</v>
       </c>
-      <c r="G83" s="13">
+      <c r="G83" s="10">
         <v>-40</v>
       </c>
       <c r="H83" s="5">
@@ -4730,7 +4729,7 @@
       <c r="F84" s="5">
         <v>30</v>
       </c>
-      <c r="G84" s="13">
+      <c r="G84" s="10">
         <v>-40</v>
       </c>
       <c r="H84" s="5">
@@ -4846,7 +4845,7 @@
         <v>10</v>
       </c>
       <c r="N86">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O86">
         <v>15</v>
@@ -4893,7 +4892,7 @@
         <v>10</v>
       </c>
       <c r="N87">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O87">
         <v>15</v>
@@ -4940,7 +4939,7 @@
         <v>10</v>
       </c>
       <c r="N88">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O88">
         <v>15</v>
@@ -4987,7 +4986,7 @@
         <v>10</v>
       </c>
       <c r="N89">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O89">
         <v>15</v>
@@ -5034,7 +5033,7 @@
         <v>10</v>
       </c>
       <c r="N90">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O90">
         <v>15</v>
@@ -5081,7 +5080,7 @@
         <v>10</v>
       </c>
       <c r="N91">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O91">
         <v>15</v>

</xml_diff>